<commit_message>
Likelihood and Impact added
Arindam had the issue where he needed to add an extra row to the csv files with an extra value. before it was just substituting an X with a value, but now it is adding a second row with all empty commas except the likehood values which will be taken from a second column.
</commit_message>
<xml_diff>
--- a/data/Values.xlsx
+++ b/data/Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pradas\PycharmProjects\ChangePropDSM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DED98A-5E81-43D7-BD86-3102698ADB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429674B1-2BF3-450F-933C-251B93E996CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="3870" windowWidth="17280" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="345" windowWidth="17280" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,10 +166,10 @@
     <t>lower the mount point and create a "bump"</t>
   </si>
   <si>
-    <t>Likehood</t>
+    <t>Impact</t>
   </si>
   <si>
-    <t>Impact</t>
+    <t>Likelihood</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:D596"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,10 +565,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>